<commit_message>
Amended import Excel function
</commit_message>
<xml_diff>
--- a/ClientContactInfo.xlsx
+++ b/ClientContactInfo.xlsx
@@ -1,12 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27316"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FECC57CE-B33B-4C3B-9523-1DF65B1D3D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -124,24 +144,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="8"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
-      <color theme="1"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,89 +172,202 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9A9A9A"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9A9A9A"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9A9A9A"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9A9A9A"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -372,29 +508,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.88"/>
-    <col customWidth="1" min="2" max="2" width="15.63"/>
-    <col customWidth="1" min="3" max="3" width="22.75"/>
-    <col customWidth="1" min="4" max="4" width="22.13"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,142 +556,123 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3">
-        <v>8809090.0</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="2">
+        <v>8809090</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3">
-        <v>98345.0</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="2">
+        <v>98345</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="3">
-        <v>78984.0</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="2">
+        <v>78984</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="3">
-        <v>78900.0</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="2">
+        <v>78900</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="3">
-        <v>67889.0</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="F6" s="2">
+        <v>67889</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>